<commit_message>
Test data, parameter sensitivity analysis, etc...
</commit_message>
<xml_diff>
--- a/TEST_DATA/FlightData_08202021_2/FlightData_08202021_2.xlsx
+++ b/TEST_DATA/FlightData_08202021_2/FlightData_08202021_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renkert2\Box\ARG_Research\QuadrotorHardware\TestFlights\FlightData_08202021_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renkert2\Documents\ARG_Research\QuadrotorOptimization\TEST_DATA\FlightData_08202021_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAECE13F-B6BC-48F9-AF88-F1B9EF9017CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8CB513-2AB9-4FBD-B5E5-EEEFDD51C574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3600" windowWidth="16440" windowHeight="28440" xr2:uid="{DCA8ECF0-3618-488F-851D-C0003A967F48}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A4:B7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,6 +468,12 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f>SUM(B1:B2)</f>
+        <v>2.2843</v>
+      </c>
+    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>

</xml_diff>